<commit_message>
Update comms & regulators
</commit_message>
<xml_diff>
--- a/research/BussOptions.xlsx
+++ b/research/BussOptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manu\Documents\461-Ass2\ence461-assignment2\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75AA40C-AE7D-4762-8FBE-12F1EA1360EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5013E93D-A8CA-4C3B-8AA0-4C9428885D14}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{758875F9-70FF-4F74-B066-49472A49A297}"/>
   </bookViews>
@@ -354,9 +354,6 @@
     <t>Asynch</t>
   </si>
   <si>
-    <t>256</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
@@ -387,9 +384,6 @@
     <t>TIA-232-F</t>
   </si>
   <si>
-    <t>(@ speed)</t>
-  </si>
-  <si>
     <t>(primary)</t>
   </si>
   <si>
@@ -439,6 +433,12 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>ISO 17897</t>
+  </si>
+  <si>
+    <t>(@ speed) m</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1074,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEA76F4-B453-4267-9CA2-EDB3FBDF0197}">
   <dimension ref="B1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1120,7 +1122,7 @@
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L2" s="14" t="s">
         <v>72</v>
@@ -1136,7 +1138,7 @@
       </c>
       <c r="P2" s="12"/>
       <c r="Q2" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R2" s="12" t="s">
         <v>82</v>
@@ -1157,28 +1159,28 @@
       </c>
       <c r="F3" s="49"/>
       <c r="G3" s="50" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="H3" s="45"/>
       <c r="I3" s="45" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J3" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="K3" s="45" t="s">
         <v>108</v>
-      </c>
-      <c r="K3" s="45" t="s">
-        <v>110</v>
       </c>
       <c r="L3" s="45"/>
       <c r="M3" s="45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="N3" s="45"/>
       <c r="O3" s="45" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="P3" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q3" s="45"/>
       <c r="R3" s="45"/>
@@ -1208,7 +1210,7 @@
         <v>39</v>
       </c>
       <c r="K4" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L4" s="22" t="s">
         <v>73</v>
@@ -1261,7 +1263,7 @@
         <v>44</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L5" s="22" t="s">
         <v>73</v>
@@ -1315,7 +1317,7 @@
         <v>39</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L6" s="22" t="s">
         <v>73</v>
@@ -1367,7 +1369,7 @@
         <v>39</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L7" s="22" t="s">
         <v>73</v>
@@ -1420,7 +1422,7 @@
         <v>44</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L8" s="27" t="s">
         <v>73</v>
@@ -1464,14 +1466,14 @@
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I9" s="20" t="s">
         <v>38</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L9" s="22" t="s">
         <v>73</v>
@@ -1522,7 +1524,7 @@
       </c>
       <c r="J10" s="30"/>
       <c r="K10" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L10" s="32" t="s">
         <v>88</v>
@@ -1571,7 +1573,7 @@
       </c>
       <c r="J11" s="30"/>
       <c r="K11" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L11" s="32" t="s">
         <v>88</v>
@@ -1624,7 +1626,7 @@
         <v>39</v>
       </c>
       <c r="K12" s="35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L12" s="37" t="s">
         <v>88</v>
@@ -1658,7 +1660,7 @@
         <v>75</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E13" s="20">
         <f>9600/1000000</f>
@@ -1678,7 +1680,7 @@
       </c>
       <c r="J13" s="20"/>
       <c r="K13" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L13" s="22" t="s">
         <v>88</v>
@@ -1835,7 +1837,7 @@
       </c>
       <c r="J16" s="17"/>
       <c r="K16" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L16" s="42" t="s">
         <v>73</v>
@@ -1884,7 +1886,7 @@
       </c>
       <c r="J17" s="17"/>
       <c r="K17" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L17" s="42" t="s">
         <v>88</v>
@@ -1916,7 +1918,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E18" s="17">
         <f>115000/1000000</f>
@@ -1936,7 +1938,7 @@
       </c>
       <c r="J18" s="17"/>
       <c r="K18" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L18" s="42" t="s">
         <v>73</v>
@@ -1965,17 +1967,17 @@
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E19" s="17">
         <f>230000/1000000</f>
         <v>0.23</v>
       </c>
       <c r="F19" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G19" s="41" t="s">
         <v>30</v>
@@ -1988,13 +1990,13 @@
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
       <c r="O19" s="42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P19" s="17"/>
       <c r="Q19" s="17"/>
       <c r="R19" s="17"/>
       <c r="S19" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="T19" s="4"/>
     </row>
@@ -2003,13 +2005,18 @@
       <c r="C20" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
+      <c r="D20" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="45">
+        <f>20000/1000000</f>
+        <v>0.02</v>
+      </c>
       <c r="F20" s="45">
         <v>2</v>
       </c>
       <c r="G20" s="46" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="H20" s="45" t="s">
         <v>41</v>
@@ -2019,7 +2026,7 @@
       </c>
       <c r="J20" s="45"/>
       <c r="K20" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L20" s="47" t="s">
         <v>88</v>
@@ -2038,58 +2045,58 @@
         <v>67</v>
       </c>
       <c r="R20" s="45"/>
-      <c r="S20" s="48" t="s">
-        <v>123</v>
+      <c r="S20" s="48">
+        <v>17</v>
       </c>
       <c r="T20" s="4"/>
     </row>
     <row r="21" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="C23" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Starting cables, connectors, update buss sheet
</commit_message>
<xml_diff>
--- a/research/BussOptions.xlsx
+++ b/research/BussOptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manu\Documents\461-Ass2\ence461-assignment2\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5013E93D-A8CA-4C3B-8AA0-4C9428885D14}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E954A7-D3F1-4AC5-BD0A-56ECF61FC0B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{758875F9-70FF-4F74-B066-49472A49A297}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="128">
   <si>
     <t>Standards</t>
   </si>
@@ -439,6 +439,18 @@
   </si>
   <si>
     <t>(@ speed) m</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Newer driver ic's allow 128 devices</t>
+  </si>
+  <si>
+    <t>128.32 Kbps</t>
+  </si>
+  <si>
+    <t>0.12832Mbps</t>
   </si>
 </sst>
 </file>
@@ -512,7 +524,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -600,6 +612,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -706,21 +755,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -754,6 +788,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1074,12 +1123,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEA76F4-B453-4267-9CA2-EDB3FBDF0197}">
   <dimension ref="B1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
@@ -1152,39 +1202,39 @@
     </row>
     <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="49"/>
-      <c r="G3" s="50" t="s">
+      <c r="F3" s="44"/>
+      <c r="G3" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45" t="s">
+      <c r="H3" s="40"/>
+      <c r="I3" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="K3" s="45" t="s">
+      <c r="K3" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45" t="s">
+      <c r="L3" s="40"/>
+      <c r="M3" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45" t="s">
+      <c r="N3" s="40"/>
+      <c r="O3" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="P3" s="45" t="s">
+      <c r="P3" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="48"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="43"/>
       <c r="T3" s="4"/>
     </row>
     <row r="4" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1542,7 +1592,7 @@
         <v>21</v>
       </c>
       <c r="Q10" s="30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R10" s="30"/>
       <c r="S10" s="33">
@@ -1552,7 +1602,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="29" t="s">
         <v>9</v>
@@ -1597,69 +1647,69 @@
       </c>
       <c r="T11" s="4"/>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="47">
         <v>0.32</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="H12" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="35" t="s">
+      <c r="I12" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="35" t="s">
+      <c r="J12" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="K12" s="35" t="s">
+      <c r="K12" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="L12" s="37" t="s">
+      <c r="L12" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="M12" s="37" t="s">
+      <c r="M12" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="N12" s="37" t="s">
+      <c r="N12" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="O12" s="35" t="s">
+      <c r="O12" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="P12" s="35" t="s">
+      <c r="P12" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="Q12" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="R12" s="35"/>
-      <c r="S12" s="38">
+      <c r="Q12" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="R12" s="47"/>
+      <c r="S12" s="50">
         <v>1024</v>
       </c>
       <c r="T12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="35" t="s">
         <v>103</v>
       </c>
       <c r="E13" s="20">
@@ -1720,10 +1770,10 @@
         <f>300/1000000</f>
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="F14" s="41" t="s">
+      <c r="F14" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="36" t="s">
         <v>55</v>
       </c>
       <c r="H14" s="17" t="s">
@@ -1736,13 +1786,13 @@
       <c r="K14" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="L14" s="42" t="s">
+      <c r="L14" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="M14" s="42" t="s">
+      <c r="M14" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="N14" s="42" t="s">
+      <c r="N14" s="37" t="s">
         <v>85</v>
       </c>
       <c r="O14" s="17"/>
@@ -1765,16 +1815,16 @@
       <c r="C15" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="38" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="17">
         <v>10</v>
       </c>
-      <c r="F15" s="41" t="s">
+      <c r="F15" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="36" t="s">
         <v>32</v>
       </c>
       <c r="H15" s="17" t="s">
@@ -1787,13 +1837,13 @@
       <c r="K15" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="L15" s="42" t="s">
+      <c r="L15" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="M15" s="42" t="s">
+      <c r="M15" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="N15" s="42" t="s">
+      <c r="N15" s="37" t="s">
         <v>85</v>
       </c>
       <c r="O15" s="17" t="s">
@@ -1809,24 +1859,26 @@
       <c r="S15" s="18">
         <v>32</v>
       </c>
-      <c r="T15" s="4"/>
+      <c r="T15" s="4" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="16" spans="2:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="38" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="17">
         <f>8000000/1000000</f>
         <v>8</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="G16" s="36" t="s">
         <v>30</v>
       </c>
       <c r="H16" s="17" t="s">
@@ -1839,13 +1891,13 @@
       <c r="K16" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="L16" s="42" t="s">
+      <c r="L16" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="M16" s="42" t="s">
+      <c r="M16" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="N16" s="42" t="s">
+      <c r="N16" s="37" t="s">
         <v>86</v>
       </c>
       <c r="O16" s="17" t="s">
@@ -1872,10 +1924,10 @@
       <c r="E17" s="17">
         <v>10</v>
       </c>
-      <c r="F17" s="41" t="s">
+      <c r="F17" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="36" t="s">
         <v>32</v>
       </c>
       <c r="H17" s="17" t="s">
@@ -1888,13 +1940,13 @@
       <c r="K17" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="L17" s="42" t="s">
+      <c r="L17" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="M17" s="42" t="s">
+      <c r="M17" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="N17" s="42" t="s">
+      <c r="N17" s="37" t="s">
         <v>85</v>
       </c>
       <c r="O17" s="17" t="s">
@@ -1917,17 +1969,17 @@
       <c r="C18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="38" t="s">
         <v>104</v>
       </c>
       <c r="E18" s="17">
         <f>115000/1000000</f>
         <v>0.115</v>
       </c>
-      <c r="F18" s="41">
+      <c r="F18" s="36">
         <v>3</v>
       </c>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="36" t="s">
         <v>32</v>
       </c>
       <c r="H18" s="17" t="s">
@@ -1940,13 +1992,13 @@
       <c r="K18" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="L18" s="42" t="s">
+      <c r="L18" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="M18" s="42" t="s">
+      <c r="M18" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="N18" s="42" t="s">
+      <c r="N18" s="37" t="s">
         <v>85</v>
       </c>
       <c r="O18" s="17" t="s">
@@ -1976,20 +2028,20 @@
         <f>230000/1000000</f>
         <v>0.23</v>
       </c>
-      <c r="F19" s="41" t="s">
+      <c r="F19" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="G19" s="41" t="s">
+      <c r="G19" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="41"/>
+      <c r="H19" s="36"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
-      <c r="O19" s="42" t="s">
+      <c r="O19" s="37" t="s">
         <v>102</v>
       </c>
       <c r="P19" s="17"/>
@@ -2002,102 +2054,132 @@
     </row>
     <row r="20" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4"/>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="45" t="s">
+      <c r="D20" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="40">
         <f>20000/1000000</f>
         <v>0.02</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F20" s="40">
         <v>2</v>
       </c>
-      <c r="G20" s="46" t="s">
+      <c r="G20" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="I20" s="45" t="s">
+      <c r="I20" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45" t="s">
+      <c r="J20" s="40"/>
+      <c r="K20" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="L20" s="47" t="s">
+      <c r="L20" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="M20" s="47" t="s">
+      <c r="M20" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="N20" s="47" t="s">
+      <c r="N20" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47" t="s">
+      <c r="O20" s="42"/>
+      <c r="P20" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="Q20" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="R20" s="45"/>
-      <c r="S20" s="48">
+      <c r="Q20" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="R20" s="40"/>
+      <c r="S20" s="43">
         <v>17</v>
       </c>
       <c r="T20" s="4"/>
     </row>
     <row r="21" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="23" spans="2:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="C23" s="9" t="s">
+      <c r="H22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="N22" t="s">
+        <v>126</v>
+      </c>
+      <c r="O22" t="s">
+        <v>127</v>
+      </c>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="2:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="D23" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>113</v>
       </c>
+      <c r="H23" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="O23"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>116</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>117</v>
       </c>
+      <c r="G24"/>
+      <c r="I24" s="2"/>
+      <c r="O24"/>
+      <c r="P24" s="1"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>118</v>
       </c>
+      <c r="G25"/>
+      <c r="I25" s="2"/>
+      <c r="O25"/>
+      <c r="P25" s="1"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>119</v>
       </c>
+      <c r="G26"/>
+      <c r="I26" s="2"/>
+      <c r="O26"/>
+      <c r="P26" s="1"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>120</v>
       </c>
+      <c r="G27"/>
+      <c r="I27" s="2"/>
+      <c r="O27"/>
+      <c r="P27" s="1"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
@@ -2210,8 +2292,8 @@
       <c r="Q33" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:T13">
-    <sortCondition descending="1" ref="E4:E13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C4:U13">
+    <sortCondition descending="1" ref="F4:F13"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" tooltip="IEC 61158" display="https://en.wikipedia.org/wiki/IEC_61158" xr:uid="{CD020E70-A3D2-48DC-8A38-D3581ADFE8A6}"/>

</xml_diff>

<commit_message>
Finish PSU section and update buss options
</commit_message>
<xml_diff>
--- a/research/BussOptions.xlsx
+++ b/research/BussOptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manu\Documents\461-Ass2\ence461-assignment2\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E954A7-D3F1-4AC5-BD0A-56ECF61FC0B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E974C0CF-D2AB-4C03-9461-4903C3E016DD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{758875F9-70FF-4F74-B066-49472A49A297}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{758875F9-70FF-4F74-B066-49472A49A297}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1121,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEA76F4-B453-4267-9CA2-EDB3FBDF0197}">
-  <dimension ref="B1:T33"/>
+  <dimension ref="B1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="R10" s="30"/>
       <c r="S10" s="33">
-        <v>1024</v>
+        <v>127</v>
       </c>
       <c r="T10" t="s">
         <v>59</v>
@@ -1698,7 +1698,7 @@
       </c>
       <c r="R12" s="47"/>
       <c r="S12" s="50">
-        <v>1024</v>
+        <v>127</v>
       </c>
       <c r="T12" t="s">
         <v>59</v>
@@ -2291,6 +2291,9 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
     </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C4:U13">
     <sortCondition descending="1" ref="F4:F13"/>

</xml_diff>